<commit_message>
Updated Input File .xlsx
</commit_message>
<xml_diff>
--- a/Halibut Model Inputs.xlsx
+++ b/Halibut Model Inputs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nmfs.local\AKC-ABL\Users\curry.cunningham\My Documents\Projects\Halibut MSE\Halibut_BioEcon\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17420" yWindow="0" windowWidth="18320" windowHeight="22520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="17415" yWindow="0" windowWidth="18315" windowHeight="22515" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Growth" sheetId="1" r:id="rId1"/>
@@ -13,8 +18,9 @@
     <sheet name="FisherySelectivity" sheetId="3" r:id="rId4"/>
     <sheet name="Control" sheetId="5" r:id="rId5"/>
     <sheet name="Fmort" sheetId="6" r:id="rId6"/>
+    <sheet name="GrowthChange" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -315,6 +321,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -646,9 +660,9 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -676,7 +690,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -690,7 +704,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
@@ -704,7 +718,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -718,7 +732,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -751,9 +765,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,7 +781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -781,7 +795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -809,16 +823,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -829,7 +843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -843,7 +857,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -854,7 +868,7 @@
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -865,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -897,13 +911,13 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -943,7 +957,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -963,7 +977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -987,7 +1001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1007,7 +1021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1027,7 +1041,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1047,7 +1061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1067,7 +1081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1087,7 +1101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1107,7 +1121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1127,7 +1141,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1161,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1186,9 +1200,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1210,7 +1224,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1239,9 +1253,9 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -1258,7 +1272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1275,7 +1289,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1292,7 +1306,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1309,7 +1323,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1326,7 +1340,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1343,7 +1357,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1360,7 +1374,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1377,7 +1391,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1394,7 +1408,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1411,7 +1425,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1428,7 +1442,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1445,7 +1459,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1462,7 +1476,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1479,7 +1493,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1496,7 +1510,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1513,7 +1527,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1530,7 +1544,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1547,7 +1561,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1564,7 +1578,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1581,7 +1595,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1598,7 +1612,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1615,7 +1629,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1632,7 +1646,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1649,7 +1663,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1666,7 +1680,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1683,7 +1697,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1700,7 +1714,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1717,7 +1731,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1734,7 +1748,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1751,7 +1765,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1768,7 +1782,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1785,7 +1799,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1802,7 +1816,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1819,7 +1833,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1836,7 +1850,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1853,7 +1867,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1870,7 +1884,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1887,7 +1901,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1904,7 +1918,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1921,7 +1935,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1938,7 +1952,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1955,7 +1969,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1972,7 +1986,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1989,7 +2003,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2006,7 +2020,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2023,7 +2037,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2040,7 +2054,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2057,7 +2071,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2074,7 +2088,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2091,7 +2105,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2128,4 +2142,18 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished input adjust and added plotting fxns
</commit_message>
<xml_diff>
--- a/Halibut Model Inputs.xlsx
+++ b/Halibut Model Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17415" yWindow="0" windowWidth="18315" windowHeight="22515" tabRatio="804" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="17415" yWindow="0" windowWidth="18315" windowHeight="22515" tabRatio="804"/>
   </bookViews>
   <sheets>
     <sheet name="Growth" sheetId="1" r:id="rId1"/>
@@ -298,7 +298,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,6 +308,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -656,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -907,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1045,16 +1046,16 @@
       <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="7">
         <v>82</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="7">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="7">
         <v>82</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="7">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">

</xml_diff>

<commit_message>
Catch and survival calculations... almost complete
</commit_message>
<xml_diff>
--- a/Halibut Model Inputs.xlsx
+++ b/Halibut Model Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17415" yWindow="0" windowWidth="18315" windowHeight="22515" tabRatio="804"/>
+    <workbookView xWindow="17415" yWindow="0" windowWidth="18315" windowHeight="22515" tabRatio="804" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Growth" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="FisherySelectivity" sheetId="3" r:id="rId4"/>
     <sheet name="Control" sheetId="5" r:id="rId5"/>
     <sheet name="Fmort" sheetId="6" r:id="rId6"/>
-    <sheet name="GrowthChange" sheetId="7" r:id="rId7"/>
+    <sheet name="Recruitment" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>Par</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>ulim</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Steepness</t>
+  </si>
+  <si>
+    <t>sigma_rec</t>
+  </si>
+  <si>
+    <t>Lognormal recruitment standard deviation (0.55-0.9)</t>
   </si>
 </sst>
 </file>
@@ -657,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1198,7 +1210,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2147,14 +2159,48 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2">
+        <v>0.75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correcting recruitment collapase effect, biomass dynamics complete
</commit_message>
<xml_diff>
--- a/Halibut Model Inputs.xlsx
+++ b/Halibut Model Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17415" yWindow="0" windowWidth="18315" windowHeight="22515" tabRatio="804" activeTab="2"/>
+    <workbookView xWindow="17415" yWindow="0" windowWidth="18315" windowHeight="22515" tabRatio="804" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Growth" sheetId="1" r:id="rId1"/>
@@ -191,9 +191,6 @@
     <t>ulim</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
     <t>Steepness</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Natural Mortality Rate (RARA_2015)</t>
+  </si>
+  <si>
+    <t>steep</t>
   </si>
 </sst>
 </file>
@@ -839,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -870,7 +870,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2164,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2183,29 +2183,29 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>0.75</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>0.9</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated file names and data import
</commit_message>
<xml_diff>
--- a/Halibut Model Inputs.xlsx
+++ b/Halibut Model Inputs.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nmfs.local\AKC-ABL\Users\curry.cunningham\My Documents\Projects\Halibut MSE\Halibut_BioEcon\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17415" yWindow="0" windowWidth="18315" windowHeight="22515" tabRatio="804" activeTab="6"/>
+    <workbookView xWindow="2620" yWindow="4440" windowWidth="25600" windowHeight="16060" tabRatio="804" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Growth" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
     <sheet name="Control" sheetId="5" r:id="rId6"/>
     <sheet name="Recruitment" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -206,7 +201,7 @@
     <t>steep</t>
   </si>
   <si>
-    <t>600 Starting biomass (millions of lbs)</t>
+    <t>1600 Starting biomass (millions of lbs)</t>
   </si>
 </sst>
 </file>
@@ -676,9 +671,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -706,7 +701,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -720,7 +715,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -734,7 +729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -748,7 +743,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -781,9 +776,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -797,7 +792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -811,7 +806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -840,15 +835,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -859,7 +854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -873,7 +868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -884,7 +879,7 @@
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -895,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -927,13 +922,13 @@
       <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -953,7 +948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -973,7 +968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -993,7 +988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -1017,7 +1012,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1037,7 +1032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1057,7 +1052,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1077,7 +1072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1097,7 +1092,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1117,7 +1112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1137,7 +1132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1157,7 +1152,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1177,7 +1172,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1210,15 +1205,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1235,858 +1230,1708 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C42">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C46">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C51">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>0.05</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:E51">
+  <conditionalFormatting sqref="B2:E101">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2112,12 +2957,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2128,23 +2973,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="4">
-        <v>600</v>
+        <v>1600</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>
@@ -2164,16 +3009,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2184,7 +3029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -2195,7 +3040,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -2206,18 +3051,23 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="3">
-        <v>10000000</v>
+        <v>30000000</v>
       </c>
       <c r="C4" s="3">
-        <v>10000000</v>
+        <v>2500000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated inputs to include simulations
</commit_message>
<xml_diff>
--- a/Halibut Model Inputs.xlsx
+++ b/Halibut Model Inputs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Par</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>1600 Starting biomass (millions of lbs)</t>
+  </si>
+  <si>
+    <t>n.sims</t>
+  </si>
+  <si>
+    <t>Number of Simulations</t>
   </si>
 </sst>
 </file>
@@ -2968,10 +2974,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3007,6 +3013,17 @@
       </c>
       <c r="C3" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>